<commit_message>
Realizando correcciones en la base de datos y finalizando Create, Read y Delete de la entidad de clientes. Posteriormente: Update
</commit_message>
<xml_diff>
--- a/documentacion/modelo_relacional.xlsx
+++ b/documentacion/modelo_relacional.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\01 Juan Diego\Trabajos extras\sancholimitada\documentacion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Documents\01 Juan Diego\Trabajos extras\sancho-limtada\documentacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="42">
   <si>
     <t>CLIENTES</t>
   </si>
@@ -144,6 +144,12 @@
   </si>
   <si>
     <t>BIGINT</t>
+  </si>
+  <si>
+    <t>1, 0</t>
+  </si>
+  <si>
+    <t>Booleano</t>
   </si>
 </sst>
 </file>
@@ -501,7 +507,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,7 +551,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>15</v>
@@ -557,7 +563,7 @@
         <v>39</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -600,7 +606,9 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
@@ -610,7 +618,9 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -642,10 +652,10 @@
         <v>2</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>24</v>
@@ -744,7 +754,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>26</v>
@@ -849,13 +859,13 @@
         <v>2</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>17</v>

</xml_diff>